<commit_message>
Finish VI documentation, implement Riccati detect check, remove strict type def
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Control_Library_CustomErrors.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Control_Library_CustomErrors.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t xml:space="preserve">JasJunk FRC Trajectory / Control Library Custom Error Codes </t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t xml:space="preserve">Riccati_DARE_N.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A, Q Matrix is not detectable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riccati_Check_Detectable.vi</t>
   </si>
 </sst>
 </file>
@@ -151,6 +157,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -349,12 +356,12 @@
   </sheetPr>
   <dimension ref="B2:E70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="148" zoomScaleNormal="148" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -680,8 +687,12 @@
         <f aca="false">B28+1</f>
         <v>514023</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
+      <c r="C29" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="E29" s="7"/>
     </row>
     <row r="30" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
remove popup debug.  Changed to error cluster and custom error codes
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Control_Library_CustomErrors.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Control_Library_CustomErrors.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
   <si>
     <t xml:space="preserve">JasJunk FRC Trajectory / Control Library Custom Error Codes </t>
   </si>
@@ -143,6 +143,69 @@
   </si>
   <si>
     <t xml:space="preserve">Riccati_Check_Detectable.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trouble creating new Kalman FIlter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KalmanFilter_New.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trouble creating new Unscented Kalman Filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UnscentedKalmanFilter_New.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trouble creating new Linear Quadratic Regulator.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinearQuadraticRegulator_New.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MeanX function reference is invalid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UnscentedKalmanFilter_New_FuncGroup.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MeanY function reference is invalid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResidX function reference is invalid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResidY function reference is invalid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddX function reference is invalid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trouble creating new Diff Drive Pose Est</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DiffDrivePoseEst_New.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trouble creating new Swerve Drive Pose Est</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SwerveDrivePoseEst_New.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H function reference is invalid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UnscentedKalmanFIlter_Correct_FuncGroup.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F function reference is invalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KalmanFilterLatencyComp_ApplyPastGlobalMeas_FuncGroup.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VisionCorrect function reference is invalid.</t>
   </si>
 </sst>
 </file>
@@ -152,7 +215,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -173,6 +236,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -236,7 +304,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -275,6 +343,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -357,11 +429,11 @@
   <dimension ref="B2:E70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="C47" activeCellId="0" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -700,8 +772,12 @@
         <f aca="false">B29+1</f>
         <v>514024</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
+      <c r="C30" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="E30" s="7"/>
     </row>
     <row r="31" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,8 +785,12 @@
         <f aca="false">B30+1</f>
         <v>514025</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="8"/>
+      <c r="C31" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="E31" s="7"/>
     </row>
     <row r="32" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -718,8 +798,12 @@
         <f aca="false">B31+1</f>
         <v>514026</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="8"/>
+      <c r="C32" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="E32" s="7"/>
     </row>
     <row r="33" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -727,8 +811,12 @@
         <f aca="false">B32+1</f>
         <v>514027</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="8"/>
+      <c r="C33" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="E33" s="7"/>
     </row>
     <row r="34" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -736,8 +824,12 @@
         <f aca="false">B33+1</f>
         <v>514028</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="8"/>
+      <c r="C34" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="E34" s="7"/>
     </row>
     <row r="35" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,8 +837,12 @@
         <f aca="false">B34+1</f>
         <v>514029</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="8"/>
+      <c r="C35" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="E35" s="7"/>
     </row>
     <row r="36" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,8 +850,12 @@
         <f aca="false">B35+1</f>
         <v>514030</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="8"/>
+      <c r="C36" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="E36" s="7"/>
     </row>
     <row r="37" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -763,8 +863,12 @@
         <f aca="false">B36+1</f>
         <v>514031</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8"/>
+      <c r="C37" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="E37" s="7"/>
     </row>
     <row r="38" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,8 +876,12 @@
         <f aca="false">B37+1</f>
         <v>514032</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="8"/>
+      <c r="C38" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="E38" s="7"/>
     </row>
     <row r="39" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,8 +889,12 @@
         <f aca="false">B38+1</f>
         <v>514033</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="8"/>
+      <c r="C39" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="E39" s="7"/>
     </row>
     <row r="40" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -790,8 +902,12 @@
         <f aca="false">B39+1</f>
         <v>514034</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="8"/>
+      <c r="C40" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="E40" s="7"/>
     </row>
     <row r="41" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -799,8 +915,12 @@
         <f aca="false">B40+1</f>
         <v>514035</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="8"/>
+      <c r="C41" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="E41" s="7"/>
     </row>
     <row r="42" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -808,8 +928,12 @@
         <f aca="false">B41+1</f>
         <v>514036</v>
       </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="8"/>
+      <c r="C42" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="E42" s="7"/>
     </row>
     <row r="43" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -817,138 +941,224 @@
         <f aca="false">B42+1</f>
         <v>514037</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="8"/>
+      <c r="C43" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="E43" s="7"/>
     </row>
     <row r="44" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="6"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="8"/>
+      <c r="B44" s="6" t="n">
+        <f aca="false">B43+1</f>
+        <v>514038</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="E44" s="7"/>
     </row>
     <row r="45" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="6"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="8"/>
+      <c r="B45" s="6" t="n">
+        <f aca="false">B44+1</f>
+        <v>514039</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="E45" s="7"/>
     </row>
     <row r="46" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="6"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="8"/>
+      <c r="B46" s="6" t="n">
+        <f aca="false">B45+1</f>
+        <v>514040</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="E46" s="7"/>
     </row>
     <row r="47" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="6"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="8"/>
+      <c r="B47" s="6" t="n">
+        <f aca="false">B46+1</f>
+        <v>514041</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="E47" s="7"/>
     </row>
     <row r="48" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="6"/>
+      <c r="B48" s="6" t="n">
+        <f aca="false">B47+1</f>
+        <v>514042</v>
+      </c>
       <c r="C48" s="7"/>
       <c r="D48" s="8"/>
       <c r="E48" s="7"/>
     </row>
     <row r="49" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="6"/>
+      <c r="B49" s="6" t="n">
+        <f aca="false">B48+1</f>
+        <v>514043</v>
+      </c>
       <c r="C49" s="7"/>
       <c r="D49" s="8"/>
       <c r="E49" s="7"/>
     </row>
     <row r="50" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="6"/>
+      <c r="B50" s="6" t="n">
+        <f aca="false">B49+1</f>
+        <v>514044</v>
+      </c>
       <c r="C50" s="7"/>
       <c r="D50" s="8"/>
       <c r="E50" s="7"/>
     </row>
     <row r="51" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="6"/>
+      <c r="B51" s="6" t="n">
+        <f aca="false">B50+1</f>
+        <v>514045</v>
+      </c>
       <c r="C51" s="7"/>
       <c r="D51" s="8"/>
       <c r="E51" s="7"/>
     </row>
     <row r="52" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="6"/>
+      <c r="B52" s="6" t="n">
+        <f aca="false">B51+1</f>
+        <v>514046</v>
+      </c>
       <c r="C52" s="7"/>
       <c r="D52" s="8"/>
       <c r="E52" s="7"/>
     </row>
     <row r="53" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="6"/>
+      <c r="B53" s="6" t="n">
+        <f aca="false">B52+1</f>
+        <v>514047</v>
+      </c>
       <c r="C53" s="7"/>
       <c r="D53" s="8"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="6"/>
+      <c r="B54" s="6" t="n">
+        <f aca="false">B53+1</f>
+        <v>514048</v>
+      </c>
       <c r="C54" s="7"/>
       <c r="D54" s="8"/>
       <c r="E54" s="7"/>
     </row>
     <row r="55" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="6"/>
+      <c r="B55" s="6" t="n">
+        <f aca="false">B54+1</f>
+        <v>514049</v>
+      </c>
       <c r="C55" s="7"/>
       <c r="D55" s="8"/>
       <c r="E55" s="7"/>
     </row>
     <row r="56" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="6"/>
+      <c r="B56" s="6" t="n">
+        <f aca="false">B55+1</f>
+        <v>514050</v>
+      </c>
       <c r="C56" s="7"/>
       <c r="D56" s="8"/>
       <c r="E56" s="7"/>
     </row>
     <row r="57" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="6"/>
+      <c r="B57" s="6" t="n">
+        <f aca="false">B56+1</f>
+        <v>514051</v>
+      </c>
       <c r="C57" s="7"/>
       <c r="D57" s="8"/>
       <c r="E57" s="7"/>
     </row>
     <row r="58" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="6"/>
+      <c r="B58" s="6" t="n">
+        <f aca="false">B57+1</f>
+        <v>514052</v>
+      </c>
       <c r="C58" s="7"/>
       <c r="D58" s="8"/>
       <c r="E58" s="7"/>
     </row>
     <row r="59" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="6"/>
+      <c r="B59" s="6" t="n">
+        <f aca="false">B58+1</f>
+        <v>514053</v>
+      </c>
       <c r="C59" s="7"/>
       <c r="D59" s="8"/>
       <c r="E59" s="7"/>
     </row>
     <row r="60" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="6"/>
+      <c r="B60" s="6" t="n">
+        <f aca="false">B59+1</f>
+        <v>514054</v>
+      </c>
       <c r="C60" s="7"/>
       <c r="D60" s="8"/>
       <c r="E60" s="7"/>
     </row>
     <row r="61" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="6"/>
+      <c r="B61" s="6" t="n">
+        <f aca="false">B60+1</f>
+        <v>514055</v>
+      </c>
       <c r="C61" s="7"/>
       <c r="D61" s="8"/>
       <c r="E61" s="7"/>
     </row>
     <row r="62" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="6"/>
+      <c r="B62" s="6" t="n">
+        <f aca="false">B61+1</f>
+        <v>514056</v>
+      </c>
       <c r="C62" s="7"/>
       <c r="D62" s="8"/>
       <c r="E62" s="7"/>
     </row>
     <row r="63" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="6"/>
+      <c r="B63" s="6" t="n">
+        <f aca="false">B62+1</f>
+        <v>514057</v>
+      </c>
       <c r="C63" s="7"/>
       <c r="D63" s="8"/>
       <c r="E63" s="7"/>
     </row>
     <row r="64" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="6"/>
+      <c r="B64" s="6" t="n">
+        <f aca="false">B63+1</f>
+        <v>514058</v>
+      </c>
       <c r="C64" s="7"/>
       <c r="D64" s="8"/>
       <c r="E64" s="7"/>
     </row>
     <row r="65" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="6"/>
+      <c r="B65" s="6" t="n">
+        <f aca="false">B64+1</f>
+        <v>514059</v>
+      </c>
       <c r="C65" s="7"/>
       <c r="D65" s="8"/>
       <c r="E65" s="7"/>

</xml_diff>

<commit_message>
Added new LQR creation routine F(A,B,,Q,R,N)
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Control_Library_CustomErrors.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Control_Library_CustomErrors.xlsx
@@ -160,7 +160,7 @@
     <t xml:space="preserve">Trouble creating new Linear Quadratic Regulator.</t>
   </si>
   <si>
-    <t xml:space="preserve">LinearQuadraticRegulator_New.vi</t>
+    <t xml:space="preserve">LinearQuadraticRegulator_New.vi, LinearQuadraticRegulator_New_N.vi</t>
   </si>
   <si>
     <t xml:space="preserve">MeanX function reference is invalid.</t>
@@ -215,7 +215,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -236,11 +236,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -304,7 +299,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -318,13 +313,25 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -337,16 +344,12 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -429,11 +432,11 @@
   <dimension ref="B2:E70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="C47" activeCellId="0" sqref="C47"/>
+      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -441,757 +444,758 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="62.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="48.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="44.49"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3" t="s">
+    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="D2" s="5"/>
     </row>
     <row r="6" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6" t="n">
+    <row r="7" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="9" t="n">
         <v>514001</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6" t="n">
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="9" t="n">
         <f aca="false">B7+1</f>
         <v>514002</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6" t="n">
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="9" t="n">
         <f aca="false">B8+1</f>
         <v>514003</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6" t="n">
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="9" t="n">
         <f aca="false">B9+1</f>
         <v>514004</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="n">
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="9" t="n">
         <f aca="false">B10+1</f>
         <v>514005</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="n">
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="9" t="n">
         <f aca="false">B11+1</f>
         <v>514006</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6" t="n">
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="9" t="n">
         <f aca="false">B12+1</f>
         <v>514007</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6" t="n">
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="9" t="n">
         <f aca="false">B13+1</f>
         <v>514008</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" s="5" customFormat="true" ht="23.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="6" t="n">
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" s="8" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="9" t="n">
         <f aca="false">B14+1</f>
         <v>514009</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="6" t="n">
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="9" t="n">
         <f aca="false">B15+1</f>
         <v>514010</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="6" t="n">
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="9" t="n">
         <f aca="false">B16+1</f>
         <v>514011</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="6" t="n">
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="9" t="n">
         <f aca="false">B17+1</f>
         <v>514012</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="6" t="n">
+    <row r="19" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="9" t="n">
         <f aca="false">B18+1</f>
         <v>514013</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="6" t="n">
+    <row r="20" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="9" t="n">
         <f aca="false">B19+1</f>
         <v>514014</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" s="5" customFormat="true" ht="34.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="6" t="n">
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" s="8" customFormat="true" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="9" t="n">
         <f aca="false">B20+1</f>
         <v>514015</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" s="5" customFormat="true" ht="23.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="6" t="n">
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" s="8" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="9" t="n">
         <f aca="false">B21+1</f>
         <v>514016</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="6" t="n">
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="9" t="n">
         <f aca="false">B22+1</f>
         <v>514017</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="6" t="n">
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="9" t="n">
         <f aca="false">B23+1</f>
         <v>514018</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="6" t="n">
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="9" t="n">
         <f aca="false">B24+1</f>
         <v>514019</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="6" t="n">
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="9" t="n">
         <f aca="false">B25+1</f>
         <v>514020</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="6" t="n">
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="9" t="n">
         <f aca="false">B26+1</f>
         <v>514021</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="9"/>
-    </row>
-    <row r="28" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="6" t="n">
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="9" t="n">
         <f aca="false">B27+1</f>
         <v>514022</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="6" t="n">
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="9" t="n">
         <f aca="false">B28+1</f>
         <v>514023</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="6" t="n">
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="9" t="n">
         <f aca="false">B29+1</f>
         <v>514024</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="6" t="n">
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="9" t="n">
         <f aca="false">B30+1</f>
         <v>514025</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="6" t="n">
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" s="8" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="9" t="n">
         <f aca="false">B31+1</f>
         <v>514026</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="6" t="n">
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="9" t="n">
         <f aca="false">B32+1</f>
         <v>514027</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="6" t="n">
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="9" t="n">
         <f aca="false">B33+1</f>
         <v>514028</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="6" t="n">
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="9" t="n">
         <f aca="false">B34+1</f>
         <v>514029</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="6" t="n">
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="9" t="n">
         <f aca="false">B35+1</f>
         <v>514030</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="6" t="n">
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="9" t="n">
         <f aca="false">B36+1</f>
         <v>514031</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="7"/>
-    </row>
-    <row r="38" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="6" t="n">
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="9" t="n">
         <f aca="false">B37+1</f>
         <v>514032</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="7"/>
-    </row>
-    <row r="39" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="6" t="n">
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="9" t="n">
         <f aca="false">B38+1</f>
         <v>514033</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="7"/>
-    </row>
-    <row r="40" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="6" t="n">
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="9" t="n">
         <f aca="false">B39+1</f>
         <v>514034</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E40" s="7"/>
-    </row>
-    <row r="41" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="6" t="n">
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="9" t="n">
         <f aca="false">B40+1</f>
         <v>514035</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="7"/>
-    </row>
-    <row r="42" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="6" t="n">
+      <c r="E41" s="10"/>
+    </row>
+    <row r="42" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="9" t="n">
         <f aca="false">B41+1</f>
         <v>514036</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E42" s="7"/>
-    </row>
-    <row r="43" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="6" t="n">
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="9" t="n">
         <f aca="false">B42+1</f>
         <v>514037</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="7"/>
-    </row>
-    <row r="44" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="6" t="n">
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="9" t="n">
         <f aca="false">B43+1</f>
         <v>514038</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="7"/>
-    </row>
-    <row r="45" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="6" t="n">
+      <c r="E44" s="10"/>
+    </row>
+    <row r="45" s="8" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="9" t="n">
         <f aca="false">B44+1</f>
         <v>514039</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E45" s="7"/>
-    </row>
-    <row r="46" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="6" t="n">
+      <c r="E45" s="10"/>
+    </row>
+    <row r="46" s="8" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="9" t="n">
         <f aca="false">B45+1</f>
         <v>514040</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E46" s="7"/>
-    </row>
-    <row r="47" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="6" t="n">
+      <c r="E46" s="10"/>
+    </row>
+    <row r="47" s="8" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="9" t="n">
         <f aca="false">B46+1</f>
         <v>514041</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E47" s="7"/>
-    </row>
-    <row r="48" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="6" t="n">
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="9" t="n">
         <f aca="false">B47+1</f>
         <v>514042</v>
       </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="7"/>
-    </row>
-    <row r="49" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="6" t="n">
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="9" t="n">
         <f aca="false">B48+1</f>
         <v>514043</v>
       </c>
-      <c r="C49" s="7"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="7"/>
-    </row>
-    <row r="50" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="6" t="n">
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="9" t="n">
         <f aca="false">B49+1</f>
         <v>514044</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="7"/>
-    </row>
-    <row r="51" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="6" t="n">
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="9" t="n">
         <f aca="false">B50+1</f>
         <v>514045</v>
       </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="7"/>
-    </row>
-    <row r="52" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="6" t="n">
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="9" t="n">
         <f aca="false">B51+1</f>
         <v>514046</v>
       </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="7"/>
-    </row>
-    <row r="53" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="6" t="n">
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="9" t="n">
         <f aca="false">B52+1</f>
         <v>514047</v>
       </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="7"/>
-    </row>
-    <row r="54" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="6" t="n">
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="9" t="n">
         <f aca="false">B53+1</f>
         <v>514048</v>
       </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="7"/>
-    </row>
-    <row r="55" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="6" t="n">
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="9" t="n">
         <f aca="false">B54+1</f>
         <v>514049</v>
       </c>
-      <c r="C55" s="7"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="7"/>
-    </row>
-    <row r="56" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="6" t="n">
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+    </row>
+    <row r="56" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="9" t="n">
         <f aca="false">B55+1</f>
         <v>514050</v>
       </c>
-      <c r="C56" s="7"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="7"/>
-    </row>
-    <row r="57" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="6" t="n">
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+    </row>
+    <row r="57" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="9" t="n">
         <f aca="false">B56+1</f>
         <v>514051</v>
       </c>
-      <c r="C57" s="7"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="7"/>
-    </row>
-    <row r="58" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="6" t="n">
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+    </row>
+    <row r="58" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="9" t="n">
         <f aca="false">B57+1</f>
         <v>514052</v>
       </c>
-      <c r="C58" s="7"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="7"/>
-    </row>
-    <row r="59" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="6" t="n">
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+    </row>
+    <row r="59" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="9" t="n">
         <f aca="false">B58+1</f>
         <v>514053</v>
       </c>
-      <c r="C59" s="7"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="7"/>
-    </row>
-    <row r="60" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="6" t="n">
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="9" t="n">
         <f aca="false">B59+1</f>
         <v>514054</v>
       </c>
-      <c r="C60" s="7"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="7"/>
-    </row>
-    <row r="61" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="6" t="n">
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+    </row>
+    <row r="61" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="9" t="n">
         <f aca="false">B60+1</f>
         <v>514055</v>
       </c>
-      <c r="C61" s="7"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="7"/>
-    </row>
-    <row r="62" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="6" t="n">
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+    </row>
+    <row r="62" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="9" t="n">
         <f aca="false">B61+1</f>
         <v>514056</v>
       </c>
-      <c r="C62" s="7"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="7"/>
-    </row>
-    <row r="63" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="6" t="n">
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+    </row>
+    <row r="63" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="9" t="n">
         <f aca="false">B62+1</f>
         <v>514057</v>
       </c>
-      <c r="C63" s="7"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="7"/>
-    </row>
-    <row r="64" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="6" t="n">
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+    </row>
+    <row r="64" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="9" t="n">
         <f aca="false">B63+1</f>
         <v>514058</v>
       </c>
-      <c r="C64" s="7"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="7"/>
-    </row>
-    <row r="65" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="6" t="n">
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+    </row>
+    <row r="65" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="9" t="n">
         <f aca="false">B64+1</f>
         <v>514059</v>
       </c>
-      <c r="C65" s="7"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="7"/>
-    </row>
-    <row r="66" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="6"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="7"/>
-    </row>
-    <row r="67" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="6"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="7"/>
-    </row>
-    <row r="68" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="6"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="7"/>
-    </row>
-    <row r="69" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="6"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="7"/>
-    </row>
-    <row r="70" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="6"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="7"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="9"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+    </row>
+    <row r="67" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="9"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+    </row>
+    <row r="68" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="9"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+    </row>
+    <row r="69" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="9"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+    </row>
+    <row r="70" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="9"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Update trajectory routines to implement #4
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Control_Library_CustomErrors.xlsx
+++ b/FRC_LV_Trajectory_Library/FRC_LabVIEW_Trajectory_Control_Library_CustomErrors.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">QuinticHermiteSplite_getControlVectorFromArrays.vi</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of control vectors must be even.</t>
+    <t xml:space="preserve">Number of control vectors must be &gt;= 2</t>
   </si>
   <si>
     <t xml:space="preserve">SplineHelp_getQuinticSplinesFromControlVectors.vi</t>
@@ -436,7 +436,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="D36" activeCellId="0" sqref="D36"/>
+      <selection pane="bottomRight" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>